<commit_message>
feat: add book structure + links digested
</commit_message>
<xml_diff>
--- a/links_to_sort.xlsx
+++ b/links_to_sort.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\r_script_codes\online_resourceR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37799D35-9175-4488-9CBD-96E208AAB4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904AA698-57E9-4337-A854-430884E310D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C803F588-0360-450B-86A1-E0442236E7D8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="923">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="1023">
   <si>
     <t>url</t>
   </si>
@@ -2759,9 +2759,6 @@
     <t>https://colinfay.me/old-faithful-express-bootstrap-webr</t>
   </si>
   <si>
-    <t>chatgpt &amp; co</t>
-  </si>
-  <si>
     <t>https://huggingface.co/chat/</t>
   </si>
   <si>
@@ -2808,6 +2805,309 @@
   </si>
   <si>
     <t>https://github.blog/2023-06-20-how-to-write-better-prompts-for-github-copilot/</t>
+  </si>
+  <si>
+    <t>Daily Papers</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/blog/document-ai</t>
+  </si>
+  <si>
+    <t>https://yjernite.github.io/lfqa.html</t>
+  </si>
+  <si>
+    <t>https://do4ds.com/</t>
+  </si>
+  <si>
+    <t>Data Science</t>
+  </si>
+  <si>
+    <t>https://pub.demo.posit.team/public/Life_Sciences_Shiny_Showcase/</t>
+  </si>
+  <si>
+    <t>Shiny</t>
+  </si>
+  <si>
+    <t>https://github.com/tangandhara/stravaDashboard/blob/main/stravaDashboard/stravaDashboard.R</t>
+  </si>
+  <si>
+    <t>https://github.com/labsyspharm/smallmoleculesuite/tree/master</t>
+  </si>
+  <si>
+    <t>https://rud.is/b/2018/04/08/dissecting-r-package-utility-belts/</t>
+  </si>
+  <si>
+    <t>R Package</t>
+  </si>
+  <si>
+    <t>https://cducloux.quarto.pub/sections/projects.html</t>
+  </si>
+  <si>
+    <t>Website Inspiration</t>
+  </si>
+  <si>
+    <t>https://github.com/ollama/ollama</t>
+  </si>
+  <si>
+    <t>Tools</t>
+  </si>
+  <si>
+    <t>https://glittr.org/contribute</t>
+  </si>
+  <si>
+    <t>https://summarize.ing/fr/pricing</t>
+  </si>
+  <si>
+    <t>https://www.tidy-finance.org/r/</t>
+  </si>
+  <si>
+    <t>https://github.com/toeverything/AFFiNE</t>
+  </si>
+  <si>
+    <t>https://github.com/Kanaries/pygwalker?tab=readme-ov-file</t>
+  </si>
+  <si>
+    <t>https://nrennie.rbind.io/talks/satrdays-london-2024/slides.html#/useful-links</t>
+  </si>
+  <si>
+    <t>https://github.com/ketchbrookanalytics/quarto-pdf-dev</t>
+  </si>
+  <si>
+    <t>https://github.com/GeostatsGuy/DataScience_Interactive_Python/blob/main/Interactive_Model_Fitting.ipynb</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2404.19756</t>
+  </si>
+  <si>
+    <t>Research Paper</t>
+  </si>
+  <si>
+    <t>https://kindxiaoming.github.io/pykan/kan.html</t>
+  </si>
+  <si>
+    <t>https://paperswithcode.com/sota</t>
+  </si>
+  <si>
+    <t>https://indiedown.cynkra.com/articles/indiedown.html</t>
+  </si>
+  <si>
+    <t>https://github.com/GeostatsGuy/DataScience_Interactive_Python/blob/main/Interactive_PCA.ipynb</t>
+  </si>
+  <si>
+    <t>https://github.com/yihui/litedown</t>
+  </si>
+  <si>
+    <t>https://colah.github.io/posts/2014-03-NN-Manifolds-Topology/</t>
+  </si>
+  <si>
+    <t>https://colah.github.io/</t>
+  </si>
+  <si>
+    <t>https://fireducks-dev.github.io/docs/benchmarks/</t>
+  </si>
+  <si>
+    <t>https://docs.sk8.inrae.fr/01-hebergement.html</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>https://github.com/Avaiga/taipy</t>
+  </si>
+  <si>
+    <t>https://github.com/OpenDevin/OpenDevin</t>
+  </si>
+  <si>
+    <t>https://training.talkpython.fm/purchase/access_code/dashboards-with-shiny-course</t>
+  </si>
+  <si>
+    <t>https://calculatingempires.net/?pos=157414.82%2C14853.40%2C14.3526</t>
+  </si>
+  <si>
+    <t>https://roadmap.sh/</t>
+  </si>
+  <si>
+    <t>https://livebook.dev/?utm_source=twitter&amp;utm_medium=social&amp;utm_content=twitter-livebook-profile</t>
+  </si>
+  <si>
+    <t>https://b-rodrigues.github.io/rix/articles/a-getting-started.html</t>
+  </si>
+  <si>
+    <t>https://www.jiddualexander.com/svg-input-generator</t>
+  </si>
+  <si>
+    <t>https://www.llmfight.club/</t>
+  </si>
+  <si>
+    <t>https://github.com/the-y-company/flexfilter?tab=readme-ov-file</t>
+  </si>
+  <si>
+    <t>https://r-packages.io/</t>
+  </si>
+  <si>
+    <t>https://joss.theoj.org/papers/10.21105/joss.06394</t>
+  </si>
+  <si>
+    <t>https://zed.dev/</t>
+  </si>
+  <si>
+    <t>https://emilhvitfeldt.github.io/ISLR-tidymodels-labs/03-linear-regression.html</t>
+  </si>
+  <si>
+    <t>https://magicinsert.github.io/</t>
+  </si>
+  <si>
+    <t>https://francoismichonneau.net/hire-me/</t>
+  </si>
+  <si>
+    <t>Personal Website</t>
+  </si>
+  <si>
+    <t>https://github.com/kennedymwavu/ambiorix-examples/tree/main/09_goals</t>
+  </si>
+  <si>
+    <t>https://theclarkeorbit.github.io/tidymodels-and-conformal-prediction.html</t>
+  </si>
+  <si>
+    <t>https://taipy.io/designer?ref=twitter&amp;utm_source=twitter&amp;utm_medium=social&amp;utm_campaign=taipy_designer&amp;utm_term=free_trial</t>
+  </si>
+  <si>
+    <t>https://github.com/advaitgosai/autocite</t>
+  </si>
+  <si>
+    <t>https://blockr-org.github.io/blockr/articles/blockr_examples.html#dynamical-systems</t>
+  </si>
+  <si>
+    <t>https://vincentarelbundock.github.io/tinytable/</t>
+  </si>
+  <si>
+    <t>https://www.cursor.com/</t>
+  </si>
+  <si>
+    <t>https://posit-conf-2024.github.io/databases/#1</t>
+  </si>
+  <si>
+    <t>Conference</t>
+  </si>
+  <si>
+    <t>https://github.com/posit-marketing/shiny-calendar</t>
+  </si>
+  <si>
+    <t>https://www.r-bloggers.com/2016/12/reactive-acronym-list-in-stratvis-a-timevis-based-shiny-app/</t>
+  </si>
+  <si>
+    <t>https://github.com/padamson/stratvis/blob/master/example/server.R</t>
+  </si>
+  <si>
+    <t>https://github.com/epi-interactive/Datatable_Overlay</t>
+  </si>
+  <si>
+    <t>https://r-wasm.github.io/quarto-drop/example.html#/title-slide</t>
+  </si>
+  <si>
+    <t>https://github.com/ddotta/ddotta</t>
+  </si>
+  <si>
+    <t>https://hutchdatascience.org/data_snacks/r_snacks/sas2r.html</t>
+  </si>
+  <si>
+    <t>https://posit.co/blog/winners-of-the-2024-shiny-contest/</t>
+  </si>
+  <si>
+    <t>https://wikicrow.ai/A1BG</t>
+  </si>
+  <si>
+    <t>https://shiny.posit.co/r/articles/improve/debugging/</t>
+  </si>
+  <si>
+    <t>https://themockup.blog/</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>https://vdsbook.com/</t>
+  </si>
+  <si>
+    <t>Book</t>
+  </si>
+  <si>
+    <t>https://rebeccabarter.com/blog/2019-08-19_purrr</t>
+  </si>
+  <si>
+    <t>https://jchiquet.github.io/MAP566/</t>
+  </si>
+  <si>
+    <t>Tutorial</t>
+  </si>
+  <si>
+    <t>https://www.pynerds.com/modules-in-python/</t>
+  </si>
+  <si>
+    <t>https://vapour.run/</t>
+  </si>
+  <si>
+    <t>https://ollama.com/blog/continue-code-assistant</t>
+  </si>
+  <si>
+    <t>https://trypear.ai/docs/quickstart</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>https://cosimameyer.com/post/git-the-perks-of-collaboration-and-version-control/</t>
+  </si>
+  <si>
+    <t>https://rtask.thinkr.fr/fr/attentes-verifiees-plongez-dans-lunivers-des-tests-unitaires-avec-expect_/#Jai_pas_le_temps_de_lire_de_quoi_ca_parle</t>
+  </si>
+  <si>
+    <t>https://rtask.thinkr.fr/fr/au-dela-des-fonctions-comment-enrichir-un-package-r-avec-des-donnees/</t>
+  </si>
+  <si>
+    <t>https://clementc.github.io/blog/2024/10/23/notes_on_PyData_Paris_2024/</t>
+  </si>
+  <si>
+    <t>https://presentofcoding.substack.com/p/github-how-to-tell-your-professional</t>
+  </si>
+  <si>
+    <t>https://pastum.anatolii.nz/</t>
+  </si>
+  <si>
+    <t>https://ml-science-book.com/causality.html</t>
+  </si>
+  <si>
+    <t>https://llamaocr.com/</t>
+  </si>
+  <si>
+    <t>https://korben.info/yt2doc-transcription-video-en-markdown.html</t>
+  </si>
+  <si>
+    <t>https://pythonds.linogaliana.fr/content/NLP/</t>
+  </si>
+  <si>
+    <t>https://pydevtools.com/blog/effective-python-developer-tooling-in-december-2024/</t>
+  </si>
+  <si>
+    <t>https://closeread.dev/</t>
+  </si>
+  <si>
+    <t>https://github.com/stackblitz-labs/bolt.diy</t>
+  </si>
+  <si>
+    <t>https://docs.astral.sh/ruff/</t>
+  </si>
+  <si>
+    <t>https://www.maturin.rs/tutorial.html</t>
+  </si>
+  <si>
+    <t>https://astral.sh/blog/uv</t>
+  </si>
+  <si>
+    <t>https://openwebui.com/</t>
   </si>
 </sst>
 </file>
@@ -2888,9 +3188,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2928,7 +3228,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3034,7 +3334,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3176,7 +3476,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3184,10 +3484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD9E5033-B6F5-4DCD-9329-62D5952EF7AA}">
-  <dimension ref="A1:G950"/>
+  <dimension ref="A1:G1041"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A805" sqref="A805"/>
+    <sheetView tabSelected="1" topLeftCell="A1017" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1042" sqref="A1042"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8268,88 +8568,1065 @@
       </c>
     </row>
     <row r="934" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A934" s="3" t="s">
-        <v>906</v>
-      </c>
+      <c r="A934" s="3"/>
     </row>
     <row r="935" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A935" s="1" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="936" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A936" s="1" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="937" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A937" s="1" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="938" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A938" s="1" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="939" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A939" s="1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="940" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A940" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="941" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A941" s="1" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="942" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A942" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="943" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A943" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="944" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A944" s="1" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="945" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A945" s="1" t="s">
         <v>916</v>
       </c>
     </row>
-    <row r="945" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A945" s="1" t="s">
+    <row r="946" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A946" s="1" t="s">
         <v>917</v>
       </c>
     </row>
-    <row r="946" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A946" s="1" t="s">
+    <row r="947" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A947" s="1" t="s">
         <v>918</v>
       </c>
     </row>
-    <row r="947" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A947" s="1" t="s">
+    <row r="948" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A948" s="1" t="s">
         <v>919</v>
       </c>
     </row>
-    <row r="948" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A948" s="1" t="s">
+    <row r="949" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A949" s="1" t="s">
         <v>920</v>
       </c>
     </row>
-    <row r="949" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A949" s="1" t="s">
+    <row r="950" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A950" s="1" t="s">
         <v>921</v>
       </c>
     </row>
-    <row r="950" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A950" s="1" t="s">
+    <row r="953" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A953" t="s">
+        <v>870</v>
+      </c>
+      <c r="B953" t="s">
         <v>922</v>
+      </c>
+      <c r="C953" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="954" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A954" t="s">
+        <v>924</v>
+      </c>
+      <c r="B954" t="s">
+        <v>922</v>
+      </c>
+      <c r="C954" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="955" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A955" t="s">
+        <v>925</v>
+      </c>
+      <c r="B955" t="s">
+        <v>922</v>
+      </c>
+      <c r="C955" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="956" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A956" t="s">
+        <v>926</v>
+      </c>
+      <c r="B956" t="s">
+        <v>927</v>
+      </c>
+      <c r="C956" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="957" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A957" t="s">
+        <v>928</v>
+      </c>
+      <c r="B957" t="s">
+        <v>929</v>
+      </c>
+      <c r="C957" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="958" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A958" t="s">
+        <v>930</v>
+      </c>
+      <c r="B958" t="s">
+        <v>929</v>
+      </c>
+      <c r="C958" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="959" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A959" t="s">
+        <v>931</v>
+      </c>
+      <c r="B959" t="s">
+        <v>929</v>
+      </c>
+      <c r="C959" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="960" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A960" t="s">
+        <v>932</v>
+      </c>
+      <c r="B960" t="s">
+        <v>933</v>
+      </c>
+      <c r="C960" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="961" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A961" t="s">
+        <v>934</v>
+      </c>
+      <c r="B961" t="s">
+        <v>935</v>
+      </c>
+      <c r="C961" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="962" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A962" t="s">
+        <v>936</v>
+      </c>
+      <c r="B962" t="s">
+        <v>937</v>
+      </c>
+      <c r="C962" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="963" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A963" t="s">
+        <v>938</v>
+      </c>
+      <c r="B963" t="s">
+        <v>937</v>
+      </c>
+      <c r="C963" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="964" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A964" t="s">
+        <v>939</v>
+      </c>
+      <c r="B964" t="s">
+        <v>937</v>
+      </c>
+      <c r="C964" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="965" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A965" t="s">
+        <v>940</v>
+      </c>
+      <c r="B965" t="s">
+        <v>937</v>
+      </c>
+      <c r="C965" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="966" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A966" t="s">
+        <v>941</v>
+      </c>
+      <c r="B966" t="s">
+        <v>937</v>
+      </c>
+      <c r="C966" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="967" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A967" t="s">
+        <v>942</v>
+      </c>
+      <c r="B967" t="s">
+        <v>937</v>
+      </c>
+      <c r="C967" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="968" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A968" t="s">
+        <v>943</v>
+      </c>
+      <c r="B968" t="s">
+        <v>937</v>
+      </c>
+      <c r="C968" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="969" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A969" t="s">
+        <v>944</v>
+      </c>
+      <c r="B969" t="s">
+        <v>937</v>
+      </c>
+      <c r="C969" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="970" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A970" t="s">
+        <v>945</v>
+      </c>
+      <c r="B970" t="s">
+        <v>937</v>
+      </c>
+      <c r="C970" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="971" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A971" t="s">
+        <v>946</v>
+      </c>
+      <c r="B971" t="s">
+        <v>947</v>
+      </c>
+      <c r="C971" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="972" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A972" t="s">
+        <v>948</v>
+      </c>
+      <c r="B972" t="s">
+        <v>937</v>
+      </c>
+      <c r="C972" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="973" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A973" t="s">
+        <v>949</v>
+      </c>
+      <c r="B973" t="s">
+        <v>947</v>
+      </c>
+      <c r="C973" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="974" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A974" t="s">
+        <v>950</v>
+      </c>
+      <c r="B974" t="s">
+        <v>937</v>
+      </c>
+      <c r="C974" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="975" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A975" t="s">
+        <v>951</v>
+      </c>
+      <c r="B975" t="s">
+        <v>937</v>
+      </c>
+      <c r="C975" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="976" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A976" t="s">
+        <v>952</v>
+      </c>
+      <c r="B976" t="s">
+        <v>937</v>
+      </c>
+      <c r="C976" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="977" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A977" t="s">
+        <v>953</v>
+      </c>
+      <c r="B977" t="s">
+        <v>947</v>
+      </c>
+      <c r="C977" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="978" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A978" t="s">
+        <v>954</v>
+      </c>
+      <c r="B978" t="s">
+        <v>947</v>
+      </c>
+      <c r="C978" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="979" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A979" t="s">
+        <v>955</v>
+      </c>
+      <c r="B979" t="s">
+        <v>937</v>
+      </c>
+      <c r="C979" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="980" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A980" t="s">
+        <v>956</v>
+      </c>
+      <c r="B980" t="s">
+        <v>937</v>
+      </c>
+      <c r="C980" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="981" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A981" t="s">
+        <v>813</v>
+      </c>
+      <c r="B981" t="s">
+        <v>937</v>
+      </c>
+      <c r="C981" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="982" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A982" t="s">
+        <v>958</v>
+      </c>
+      <c r="B982" t="s">
+        <v>937</v>
+      </c>
+      <c r="C982" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="983" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A983" t="s">
+        <v>959</v>
+      </c>
+      <c r="B983" t="s">
+        <v>937</v>
+      </c>
+      <c r="C983" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="984" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A984" t="s">
+        <v>960</v>
+      </c>
+      <c r="B984" t="s">
+        <v>929</v>
+      </c>
+      <c r="C984" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="985" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A985" t="s">
+        <v>961</v>
+      </c>
+      <c r="B985" t="s">
+        <v>937</v>
+      </c>
+      <c r="C985" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="986" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A986" t="s">
+        <v>962</v>
+      </c>
+      <c r="B986" t="s">
+        <v>937</v>
+      </c>
+      <c r="C986" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="987" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A987" t="s">
+        <v>963</v>
+      </c>
+      <c r="B987" t="s">
+        <v>937</v>
+      </c>
+      <c r="C987" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="988" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A988" t="s">
+        <v>964</v>
+      </c>
+      <c r="B988" t="s">
+        <v>937</v>
+      </c>
+      <c r="C988" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="989" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A989" t="s">
+        <v>965</v>
+      </c>
+      <c r="B989" t="s">
+        <v>937</v>
+      </c>
+      <c r="C989" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="990" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A990" t="s">
+        <v>966</v>
+      </c>
+      <c r="B990" t="s">
+        <v>937</v>
+      </c>
+      <c r="C990" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="991" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A991" t="s">
+        <v>967</v>
+      </c>
+      <c r="B991" t="s">
+        <v>937</v>
+      </c>
+      <c r="C991" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="992" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A992" t="s">
+        <v>968</v>
+      </c>
+      <c r="B992" t="s">
+        <v>937</v>
+      </c>
+      <c r="C992" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="993" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A993" t="s">
+        <v>969</v>
+      </c>
+      <c r="B993" t="s">
+        <v>947</v>
+      </c>
+      <c r="C993" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="994" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A994" t="s">
+        <v>970</v>
+      </c>
+      <c r="B994" t="s">
+        <v>937</v>
+      </c>
+      <c r="C994" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="995" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A995" t="s">
+        <v>971</v>
+      </c>
+      <c r="B995" t="s">
+        <v>927</v>
+      </c>
+      <c r="C995" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="996" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A996" t="s">
+        <v>972</v>
+      </c>
+      <c r="B996" t="s">
+        <v>937</v>
+      </c>
+      <c r="C996" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="997" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A997" t="s">
+        <v>887</v>
+      </c>
+      <c r="B997" t="s">
+        <v>937</v>
+      </c>
+      <c r="C997" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="998" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A998" t="s">
+        <v>973</v>
+      </c>
+      <c r="B998" t="s">
+        <v>974</v>
+      </c>
+      <c r="C998" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="999" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A999" t="s">
+        <v>975</v>
+      </c>
+      <c r="B999" t="s">
+        <v>937</v>
+      </c>
+      <c r="C999" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1000" t="s">
+        <v>976</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1000" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1001" t="s">
+        <v>977</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>937</v>
+      </c>
+      <c r="C1001" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1002" t="s">
+        <v>978</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>937</v>
+      </c>
+      <c r="C1002" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1003" t="s">
+        <v>979</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>937</v>
+      </c>
+      <c r="C1003" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1004" t="s">
+        <v>980</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>937</v>
+      </c>
+      <c r="C1004" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1005" t="s">
+        <v>981</v>
+      </c>
+      <c r="B1005" t="s">
+        <v>937</v>
+      </c>
+      <c r="C1005" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1006" t="s">
+        <v>982</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>983</v>
+      </c>
+      <c r="C1006" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1007" t="s">
+        <v>984</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>929</v>
+      </c>
+      <c r="C1007" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1008" t="s">
+        <v>985</v>
+      </c>
+      <c r="B1008" t="s">
+        <v>929</v>
+      </c>
+      <c r="C1008" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1009" t="s">
+        <v>986</v>
+      </c>
+      <c r="B1009" t="s">
+        <v>929</v>
+      </c>
+      <c r="C1009" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1010" t="s">
+        <v>987</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>937</v>
+      </c>
+      <c r="C1010" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1011" t="s">
+        <v>988</v>
+      </c>
+      <c r="B1011" t="s">
+        <v>937</v>
+      </c>
+      <c r="C1011" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1012" t="s">
+        <v>989</v>
+      </c>
+      <c r="B1012" t="s">
+        <v>937</v>
+      </c>
+      <c r="C1012" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1013" t="s">
+        <v>990</v>
+      </c>
+      <c r="B1013" t="s">
+        <v>927</v>
+      </c>
+      <c r="C1013" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1014" t="s">
+        <v>991</v>
+      </c>
+      <c r="B1014" t="s">
+        <v>929</v>
+      </c>
+      <c r="C1014" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1015" t="s">
+        <v>992</v>
+      </c>
+      <c r="B1015" t="s">
+        <v>937</v>
+      </c>
+      <c r="C1015" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1016" t="s">
+        <v>993</v>
+      </c>
+      <c r="B1016" t="s">
+        <v>929</v>
+      </c>
+      <c r="C1016" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1017" t="s">
+        <v>994</v>
+      </c>
+      <c r="B1017" t="s">
+        <v>995</v>
+      </c>
+      <c r="C1017" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1018" t="s">
+        <v>996</v>
+      </c>
+      <c r="B1018" t="s">
+        <v>997</v>
+      </c>
+      <c r="C1018" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1019" t="s">
+        <v>998</v>
+      </c>
+      <c r="B1019" t="s">
+        <v>995</v>
+      </c>
+      <c r="C1019" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1020" t="s">
+        <v>999</v>
+      </c>
+      <c r="B1020" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C1020" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1021" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B1021" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C1021" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1022" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B1022" t="s">
+        <v>937</v>
+      </c>
+      <c r="C1022" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1023" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B1023" t="s">
+        <v>995</v>
+      </c>
+      <c r="C1023" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1024" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B1024" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C1024" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1025" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B1025" t="s">
+        <v>995</v>
+      </c>
+      <c r="C1025" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1026" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B1026" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C1026" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1027" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B1027" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C1027" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1028" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B1028" t="s">
+        <v>995</v>
+      </c>
+      <c r="C1028" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1029" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B1029" t="s">
+        <v>995</v>
+      </c>
+      <c r="C1029" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1030" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B1030" t="s">
+        <v>995</v>
+      </c>
+      <c r="C1030" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1031" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B1031" t="s">
+        <v>997</v>
+      </c>
+      <c r="C1031" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1032" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B1032" t="s">
+        <v>937</v>
+      </c>
+      <c r="C1032" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1033" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B1033" t="s">
+        <v>995</v>
+      </c>
+      <c r="C1033" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1034" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B1034" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C1034" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1035" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B1035" t="s">
+        <v>995</v>
+      </c>
+      <c r="C1035" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1036" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B1036" t="s">
+        <v>995</v>
+      </c>
+      <c r="C1036" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1037" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B1037" t="s">
+        <v>937</v>
+      </c>
+      <c r="C1037" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1038" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B1038" t="s">
+        <v>937</v>
+      </c>
+      <c r="C1038" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1039" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B1039" t="s">
+        <v>937</v>
+      </c>
+      <c r="C1039" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1040" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B1040" t="s">
+        <v>937</v>
+      </c>
+      <c r="C1040" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1041" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B1041" t="s">
+        <v>937</v>
+      </c>
+      <c r="C1041" t="s">
+        <v>923</v>
       </c>
     </row>
   </sheetData>
@@ -8560,8 +9837,12 @@
     <hyperlink ref="A948" r:id="rId203" xr:uid="{2170731D-6F29-4EB2-BB83-16FA35BC4B68}"/>
     <hyperlink ref="A949" r:id="rId204" xr:uid="{9A4DC74C-23BB-4CB1-A0D4-A773B0F35044}"/>
     <hyperlink ref="A950" r:id="rId205" xr:uid="{F7BC10C8-B75B-4E21-9931-6F3FE0CEBB58}"/>
+    <hyperlink ref="A1037" r:id="rId206" xr:uid="{6A06F517-32EB-4DDD-8742-2B62FB5A66CD}"/>
+    <hyperlink ref="A1038" r:id="rId207" xr:uid="{27EBB1A5-135C-4E38-A0F9-EED9B0F24648}"/>
+    <hyperlink ref="A1039" r:id="rId208" xr:uid="{FF360C75-4C36-4DE0-A5B1-38E63851E626}"/>
+    <hyperlink ref="A1041" r:id="rId209" xr:uid="{EE5E9383-5BA9-4980-A0D7-8CAE0DD2C16E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId206"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId210"/>
 </worksheet>
 </file>
</xml_diff>